<commit_message>
changes from a long time ago
</commit_message>
<xml_diff>
--- a/Gegenbauer/params.xlsx
+++ b/Gegenbauer/params.xlsx
@@ -629,7 +629,7 @@
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M1048576"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,15 +681,6 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="K3">
-        <v>490</v>
-      </c>
-      <c r="L3">
-        <v>6</v>
-      </c>
-      <c r="M3">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -704,15 +695,6 @@
       <c r="D4">
         <v>5</v>
       </c>
-      <c r="K4">
-        <v>1064</v>
-      </c>
-      <c r="L4">
-        <v>8</v>
-      </c>
-      <c r="M4">
-        <v>7</v>
-      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -727,15 +709,6 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="K5">
-        <v>616</v>
-      </c>
-      <c r="L5">
-        <v>8</v>
-      </c>
-      <c r="M5">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -751,13 +724,13 @@
         <v>4</v>
       </c>
       <c r="K6">
-        <v>828</v>
+        <v>112</v>
       </c>
       <c r="L6">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -774,13 +747,13 @@
         <v>4</v>
       </c>
       <c r="K7">
-        <v>1470</v>
+        <v>180</v>
       </c>
       <c r="L7">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="M7">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -797,13 +770,13 @@
         <v>3</v>
       </c>
       <c r="K8">
-        <v>1274</v>
+        <v>140</v>
       </c>
       <c r="L8">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="M8">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -820,13 +793,13 @@
         <v>3</v>
       </c>
       <c r="K9">
-        <v>2058</v>
+        <v>308</v>
       </c>
       <c r="L9">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M9">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -843,13 +816,13 @@
         <v>6</v>
       </c>
       <c r="K10">
-        <v>1680</v>
+        <v>532</v>
       </c>
       <c r="L10">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M10">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -866,13 +839,13 @@
         <v>6</v>
       </c>
       <c r="K11">
-        <v>1022</v>
+        <v>812</v>
       </c>
       <c r="L11">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="M11">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -888,15 +861,6 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="K12">
-        <v>1456</v>
-      </c>
-      <c r="L12">
-        <v>16</v>
-      </c>
-      <c r="M12">
-        <v>7</v>
-      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -911,15 +875,6 @@
       <c r="D13">
         <v>3</v>
       </c>
-      <c r="K13">
-        <v>882</v>
-      </c>
-      <c r="L13">
-        <v>14</v>
-      </c>
-      <c r="M13">
-        <v>7</v>
-      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -934,15 +889,6 @@
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="K14">
-        <v>1400</v>
-      </c>
-      <c r="L14">
-        <v>20</v>
-      </c>
-      <c r="M14">
-        <v>7</v>
-      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1311,6 +1257,15 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
+      </c>
+      <c r="B41">
+        <v>812</v>
+      </c>
+      <c r="C41">
+        <v>29</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>